<commit_message>
自动更新Excel文件 - 2025-10-06 23:11:54
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20250930</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20250929</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20250929</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20250929</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20250929</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20250930</v>
+        <v>20251007</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20250929</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20250929</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20250929</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20250929</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20250929</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20250929</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20250929</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20250929</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20250929</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20250929</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20250929</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20250929</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20250929</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20250930</v>
+        <v>20251007</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20250928</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20250928</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20250928</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20250930</v>
+        <v>20251007</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20250928</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20250928</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20250928</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20250929</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20250929</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20250929</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20250929</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20250929</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20250930</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20250930</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20250930</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20250930</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20250930</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20250930</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20250930</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251002</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-07 23:11:50
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20250930</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20250929</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20250929</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20250929</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20250929</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20250929</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20250929</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20250929</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20250929</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20250929</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20250929</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20250929</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20250929</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20250929</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20250929</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20250929</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20250929</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20250929</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20250929</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20250929</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20250929</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20250929</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20250929</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20250930</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20250930</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20250930</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20250930</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20250930</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20250930</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20250930</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251002</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-08 23:11:47
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20250930</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20250930</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20250930</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20250930</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20250930</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20250930</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20250930</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20250930</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251002</v>
+        <v>20251009</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-09 23:11:46
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-10 23:12:07
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-11 23:10:42
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251002</v>
+        <v>20251012</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-13 23:11:43
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-14 23:11:51
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-15 23:11:42
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251009</v>
+        <v>20251016</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-16 23:11:46
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-17 23:11:29
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-18 23:11:15
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-19 23:11:28
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-20 23:12:03
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-21 23:12:26
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251012</v>
+        <v>20251022</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-22 23:11:00
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251016</v>
+        <v>20251023</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-23 23:11:37
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-24 23:12:08
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-25 23:11:14
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-26 23:11:58
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-27 23:12:01
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-28 23:12:15
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-29 23:12:35
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251023</v>
+        <v>20251030</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-30 23:11:54
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-10-31 23:12:23
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251022</v>
+        <v>20251101</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-01 23:12:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-02 23:11:34
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-03 23:12:17
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-04 23:14:43
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-05 23:12:38
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251030</v>
+        <v>20251106</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-06 23:12:06
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-07 23:11:50
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-08 23:11:36
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-09 23:11:52
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-10 23:12:38
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251101</v>
+        <v>20251111</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-11 23:20:55
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-12 23:12:50
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251106</v>
+        <v>20251113</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-13 23:12:28
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-14 23:12:17
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-15 23:12:09
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-16 23:11:50
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-17 23:12:11
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-18 23:12:19
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-19 23:12:52
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251113</v>
+        <v>20251120</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-20 23:12:25
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251111</v>
+        <v>20251121</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-21 23:12:06
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-22 23:12:25
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-23 23:11:59
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-24 23:12:40
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-25 23:12:40
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-26 23:12:23
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251120</v>
+        <v>20251127</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-27 23:12:14
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-28 23:12:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-29 23:12:09
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-11-30 23:12:05
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251121</v>
+        <v>20251201</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-01 23:12:39
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-02 23:12:27
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-03 23:11:09
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251127</v>
+        <v>20251204</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-04 23:13:00
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-05 23:13:19
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-06 23:12:13
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-07 23:11:57
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-08 23:13:09
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-09 23:12:58
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-10 23:11:58
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251204</v>
+        <v>20251211</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251201</v>
+        <v>20251211</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-11 23:13:27
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-12 23:13:42
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-13 23:12:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-14 23:12:18
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-15 23:14:01
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-16 23:13:01
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-17 23:13:33
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251211</v>
+        <v>20251218</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-18 23:13:57
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-19 23:13:30
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-20 23:12:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251211</v>
+        <v>20251221</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-21 23:12:39
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-22 23:13:15
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-23 23:12:56
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-24 23:13:08
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251218</v>
+        <v>20251225</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-25 23:13:27
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-26 23:13:31
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-27 23:12:33
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-28 23:13:07
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-29 23:13:19
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-30 23:12:56
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251221</v>
+        <v>20251231</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2025-12-31 23:13:24
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251225</v>
+        <v>20260101</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-01 23:13:39
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-02 23:13:02
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-03 23:13:25
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-04 23:13:20
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-05 23:13:34
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-06 23:22:43
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-07 23:13:54
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260101</v>
+        <v>20260108</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-08 23:12:59
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-09 23:13:36
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251231</v>
+        <v>20260110</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-10 23:13:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-11 23:13:18
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-12 23:11:58
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-13 23:14:05
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-14 23:12:40
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260108</v>
+        <v>20260115</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-15 23:14:11
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-16 23:13:33
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-17 23:13:10
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-18 23:13:27
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-19 23:14:04
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20260110</v>
+        <v>20260120</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-20 23:14:30
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-21 23:18:22
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260115</v>
+        <v>20260122</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-22 23:14:28
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-23 23:14:53
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-24 23:13:39
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20260124</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20260124</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20260124</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20260124</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20260124</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20260124</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20260124</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20260124</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20260124</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20260124</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20260124</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20260124</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20260124</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-25 23:13:53
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20260124</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20260124</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20260124</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20260124</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20260112</v>
+        <v>20260126</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20260124</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20260124</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20260124</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20260124</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20260124</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20260124</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20260124</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20260124</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20260116</v>
+        <v>20260126</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20260124</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20260119</v>
+        <v>20260126</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - 2026-01-26 23:24:08
</commit_message>
<xml_diff>
--- a/yxc.xlsx
+++ b/yxc.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
- 